<commit_message>
model_small = mit 75 Haselnüssen
</commit_message>
<xml_diff>
--- a/input_nuts-small.xlsx
+++ b/input_nuts-small.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a631459e6cf3f3cb/Uni/Master/2021_ss_decision-analysis/Agroforestry/Nuts_and_chicken/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="462" documentId="8_{3568966E-F10A-4A87-8770-2C8F7733F410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95D8A08C-E6DE-4CA2-BE66-DE9176101984}"/>
+  <xr:revisionPtr revIDLastSave="479" documentId="8_{3568966E-F10A-4A87-8770-2C8F7733F410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3BEDBC7-FEA3-43F1-B289-17F8B5DCB489}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{374AAA1E-B073-4CF1-B979-99CE47E0D28D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{374AAA1E-B073-4CF1-B979-99CE47E0D28D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -294,12 +294,6 @@
     <t>Nut Harvest hours</t>
   </si>
   <si>
-    <t>work_irrigation_installation_annual</t>
-  </si>
-  <si>
-    <t>Annual installation of irrigation work</t>
-  </si>
-  <si>
     <t>tree_planting_hours</t>
   </si>
   <si>
@@ -337,6 +331,12 @@
   </si>
   <si>
     <t>Cost for Water trailer in €</t>
+  </si>
+  <si>
+    <t>work_per_trailer</t>
+  </si>
+  <si>
+    <t>Hours for refilling the Trailor</t>
   </si>
 </sst>
 </file>
@@ -352,7 +352,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -362,12 +362,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -384,13 +378,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -708,7 +701,7 @@
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,29 +823,29 @@
         <v>53</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="5">
+    </row>
+    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="1">
         <v>6</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="5">
-        <v>9</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="G6" s="5" t="s">
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -899,7 +892,7 @@
         <v>84</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -953,7 +946,7 @@
         <v>18</v>
       </c>
       <c r="B11" s="1">
-        <v>350</v>
+        <v>400</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>8</v>
@@ -976,7 +969,7 @@
         <v>19</v>
       </c>
       <c r="B12" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>8</v>
@@ -1040,50 +1033,50 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" s="1">
+        <v>300</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="1">
+        <v>500</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B15" s="5">
-        <v>300</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="5">
-        <v>500</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="5" t="s">
+      <c r="B16" s="1">
+        <v>250</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="1">
+        <v>350</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G15" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="G16" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="B16" s="5">
-        <v>250</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="5">
-        <v>350</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1211,13 +1204,13 @@
         <v>28</v>
       </c>
       <c r="B23" s="1">
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D23" s="1">
-        <v>1000</v>
+        <v>1100</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>9</v>
@@ -1298,110 +1291,110 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+    <row r="27" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="1">
+        <v>5000</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" s="1">
+        <v>6000</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="1">
+        <v>6000</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B27" s="5">
-        <v>2000</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="5">
-        <v>5000</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B28" s="5">
-        <v>6000</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="5">
-        <v>6000</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B29" s="4">
-        <v>12</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="4">
-        <v>20</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>87</v>
+      <c r="G28" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="1">
+        <v>2</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B30" s="1">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D30" s="1">
-        <v>4</v>
+        <v>150</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="B31" s="1">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D31" s="1">
-        <v>150</v>
+        <v>3</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Vector instead of values
</commit_message>
<xml_diff>
--- a/input_nuts-small.xlsx
+++ b/input_nuts-small.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a631459e6cf3f3cb/Uni/Master/2021_ss_decision-analysis/Agroforestry/Nuts_and_chicken/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9af5f397540487a4/R/Nuts_and_chicken/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="479" documentId="8_{3568966E-F10A-4A87-8770-2C8F7733F410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3BEDBC7-FEA3-43F1-B289-17F8B5DCB489}"/>
+  <xr:revisionPtr revIDLastSave="482" documentId="8_{3568966E-F10A-4A87-8770-2C8F7733F410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{896D266E-DD8D-4534-9F96-39B7D3965F2A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{374AAA1E-B073-4CF1-B979-99CE47E0D28D}"/>
   </bookViews>
@@ -701,7 +701,7 @@
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1537,13 +1537,13 @@
         <v>41</v>
       </c>
       <c r="B38" s="1">
-        <v>56000</v>
+        <v>180</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D38" s="1">
-        <v>60000</v>
+        <v>220</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>9</v>

</xml_diff>